<commit_message>
Complete top 10 taxa of ITS
</commit_message>
<xml_diff>
--- a/ITS_analysis/FungalTop10Taxa.xlsx
+++ b/ITS_analysis/FungalTop10Taxa.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arifinabintarti/Documents/Parent/apple_replant/ITS_analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D89FEA22-2110-9548-8015-8F187F790D5C}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EA0A153-B005-FD41-8C51-E9CBC21D6239}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{B0C6C659-BE19-4A4E-9D21-C411D8A65FBB}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Fungal" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1503" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1713" uniqueCount="210">
   <si>
     <t>Fungal analysis</t>
   </si>
@@ -593,13 +593,224 @@
   </si>
   <si>
     <t>Fusarium oxysporum</t>
+  </si>
+  <si>
+    <t>This fungi is known as yeast and soil analysis of the site shown high abundance of this fungi. Previous study reported that this genus presents in a significant proportion of fungal communities in the forest soil and litter.</t>
+  </si>
+  <si>
+    <r>
+      <t>The Pezizales can be </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>saprobic, mycorrhizal</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF222222"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>, or parasitic on plants.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Helotiales contains more than 3000 species. This group mostly live as saprophytic fungi that contribute to the content of soil organic matter. But some members of the group are important plant pathogens (e.g. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Sclerotinia</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Sclerotium</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>).</t>
+    </r>
+  </si>
+  <si>
+    <t>Approximately 500 species belong to this group. The majority of the members are saprotrophs, some species have been reported as ectomycorrhizal. But most species of the group are poorly studied.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Ascomycota is the largest group of fungi, therefore it is highly abundant in the study also in some previous study. Most plant pathogens are under this group, e.g. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Fusarium</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Most species of this group contribute in the decaying of cellulose like died wood. Some are pathogenic fungi that can cause plant rots. </t>
+  </si>
+  <si>
+    <t>The fungi live as saprotrophic on decaying wood.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Most of </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Clavaria </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>species are saprotrophic fungi.</t>
+    </r>
+  </si>
+  <si>
+    <t>Serendipitaceae includes endophytic fungi and  ectomycorrhizal fungi. 
+The group has beneficial effects on host plants, such as enhance plant tolerance against abiotic and pathogen stresses.</t>
+  </si>
+  <si>
+    <t>The member of the group are actually fungal-like microorganisms. It is included under Fungal Kingdom because of some similar characteristics.</t>
+  </si>
+  <si>
+    <t>A broad range group, including Helotiales which can be plant pathogen, mycorrhyzae, or saprobes.</t>
+  </si>
+  <si>
+    <t>Tremellomycetes consists of parasitic or simbiotic fungi and some are saprotrophic.</t>
+  </si>
+  <si>
+    <t>Mortierella lives as saprotrophs in the soil and contributes for soil organic matter.</t>
+  </si>
+  <si>
+    <t>This group of fungi consists of more than 700 species that contain 
+plant- pathogenic and saprotrophic species.</t>
+  </si>
+  <si>
+    <t>Species that belong to Hyaloscyphaceae live as saprophytic fungi.</t>
+  </si>
+  <si>
+    <t>The members of Sporidiobolales are non-phytoparasitic fungi.</t>
+  </si>
+  <si>
+    <t>The members are parasitic or plant-pathogenic fungi and also
+ saprotrophs.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Many strains of </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>F. oxysporum</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> are plant pathogens.</t>
+    </r>
+  </si>
+  <si>
+    <t>See description above.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The Nectriaceae includes numerous of plant pathogens, e.g. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Fusarium</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>The species has big fruiting body and lives as saprobic on the dead
+ wood</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="7">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -637,6 +848,16 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF222222"/>
+      <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri (Body)"/>
     </font>
   </fonts>
   <fills count="2">
@@ -782,7 +1003,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -842,6 +1063,60 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1158,8 +1433,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8EADCF3-83B0-A14B-B15E-29B4A2733B60}">
   <dimension ref="A1:J216"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K208" sqref="K208"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F224" sqref="F224"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1173,7 +1448,7 @@
     <col min="7" max="7" width="14.1640625" style="11" customWidth="1"/>
     <col min="8" max="8" width="19.83203125" style="11" customWidth="1"/>
     <col min="9" max="9" width="14" style="11" customWidth="1"/>
-    <col min="10" max="10" width="16" style="11" customWidth="1"/>
+    <col min="10" max="10" width="59.83203125" style="11" customWidth="1"/>
     <col min="11" max="16384" width="10.83203125" style="11"/>
   </cols>
   <sheetData>
@@ -1301,63 +1576,69 @@
       <c r="I7" s="12">
         <v>18.77</v>
       </c>
-      <c r="J7" s="15"/>
-    </row>
-    <row r="8" spans="1:10">
+      <c r="J7" s="15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="64">
       <c r="A8" s="13"/>
-      <c r="B8" s="13" t="s">
+      <c r="B8" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="13" t="s">
+      <c r="D8" s="35" t="s">
         <v>46</v>
       </c>
-      <c r="E8" s="13" t="s">
+      <c r="E8" s="35" t="s">
         <v>47</v>
       </c>
-      <c r="F8" s="13" t="s">
+      <c r="F8" s="35" t="s">
         <v>48</v>
       </c>
-      <c r="G8" s="18" t="s">
+      <c r="G8" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="H8" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="I8" s="13">
+      <c r="H8" s="37" t="s">
+        <v>9</v>
+      </c>
+      <c r="I8" s="35">
         <v>10.27</v>
       </c>
-      <c r="J8" s="16"/>
-    </row>
-    <row r="9" spans="1:10">
-      <c r="A9" s="13"/>
-      <c r="B9" s="13" t="s">
+      <c r="J8" s="38" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" s="41" customFormat="1" ht="64">
+      <c r="A9" s="35"/>
+      <c r="B9" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="13" t="s">
+      <c r="D9" s="35" t="s">
         <v>58</v>
       </c>
-      <c r="E9" s="23" t="s">
+      <c r="E9" s="39" t="s">
         <v>16</v>
       </c>
-      <c r="F9" s="23" t="s">
-        <v>9</v>
-      </c>
-      <c r="G9" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="H9" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="I9" s="13">
+      <c r="F9" s="39" t="s">
+        <v>9</v>
+      </c>
+      <c r="G9" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="H9" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="I9" s="35">
         <v>6.21</v>
       </c>
-      <c r="J9" s="16"/>
+      <c r="J9" s="38" t="s">
+        <v>191</v>
+      </c>
     </row>
     <row r="10" spans="1:10">
       <c r="A10" s="13"/>
@@ -1385,35 +1666,39 @@
       <c r="I10" s="13">
         <v>5.58</v>
       </c>
-      <c r="J10" s="16"/>
-    </row>
-    <row r="11" spans="1:10">
-      <c r="A11" s="13"/>
-      <c r="B11" s="13" t="s">
+      <c r="J10" s="49" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" s="41" customFormat="1" ht="32">
+      <c r="A11" s="35"/>
+      <c r="B11" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="13" t="s">
+      <c r="C11" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="D11" s="23" t="s">
+      <c r="D11" s="39" t="s">
         <v>70</v>
       </c>
-      <c r="E11" s="13" t="s">
+      <c r="E11" s="35" t="s">
         <v>40</v>
       </c>
-      <c r="F11" s="13" t="s">
+      <c r="F11" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="G11" s="19" t="s">
+      <c r="G11" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="H11" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="I11" s="13">
+      <c r="H11" s="37" t="s">
+        <v>9</v>
+      </c>
+      <c r="I11" s="35">
         <v>4.51</v>
       </c>
-      <c r="J11" s="16"/>
+      <c r="J11" s="38" t="s">
+        <v>201</v>
+      </c>
     </row>
     <row r="12" spans="1:10">
       <c r="A12" s="13"/>
@@ -1441,7 +1726,9 @@
       <c r="I12" s="13">
         <v>2.4700000000000002</v>
       </c>
-      <c r="J12" s="16"/>
+      <c r="J12" s="16" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="13" spans="1:10">
       <c r="A13" s="13"/>
@@ -1469,35 +1756,39 @@
       <c r="I13" s="13">
         <v>2.12</v>
       </c>
-      <c r="J13" s="16"/>
-    </row>
-    <row r="14" spans="1:10">
-      <c r="A14" s="13"/>
-      <c r="B14" s="13" t="s">
+      <c r="J13" s="16" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" s="41" customFormat="1" ht="64">
+      <c r="A14" s="35"/>
+      <c r="B14" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="13" t="s">
+      <c r="C14" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="D14" s="24" t="s">
-        <v>9</v>
-      </c>
-      <c r="E14" s="24" t="s">
-        <v>9</v>
-      </c>
-      <c r="F14" s="24" t="s">
-        <v>9</v>
-      </c>
-      <c r="G14" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="H14" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="I14" s="13">
+      <c r="D14" s="43" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" s="43" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" s="43" t="s">
+        <v>9</v>
+      </c>
+      <c r="G14" s="44" t="s">
+        <v>9</v>
+      </c>
+      <c r="H14" s="37" t="s">
+        <v>9</v>
+      </c>
+      <c r="I14" s="35">
         <v>1.89</v>
       </c>
-      <c r="J14" s="16"/>
+      <c r="J14" s="38" t="s">
+        <v>193</v>
+      </c>
     </row>
     <row r="15" spans="1:10">
       <c r="A15" s="13"/>
@@ -1525,7 +1816,9 @@
       <c r="I15" s="13">
         <v>1.65</v>
       </c>
-      <c r="J15" s="16"/>
+      <c r="J15" s="16" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="16" spans="1:10">
       <c r="A16" s="14"/>
@@ -1553,7 +1846,9 @@
       <c r="I16" s="14">
         <v>1.57</v>
       </c>
-      <c r="J16" s="17"/>
+      <c r="J16" s="17" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="17" spans="1:10">
       <c r="A17" s="13" t="s">
@@ -1583,7 +1878,9 @@
       <c r="I17" s="24">
         <v>25.28</v>
       </c>
-      <c r="J17" s="16"/>
+      <c r="J17" s="16" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="18" spans="1:10">
       <c r="A18" s="13"/>
@@ -1611,35 +1908,39 @@
       <c r="I18" s="24">
         <v>17.64</v>
       </c>
-      <c r="J18" s="16"/>
-    </row>
-    <row r="19" spans="1:10">
-      <c r="A19" s="13"/>
-      <c r="B19" s="13" t="s">
+      <c r="J18" s="16" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" s="41" customFormat="1" ht="80">
+      <c r="A19" s="35"/>
+      <c r="B19" s="35" t="s">
         <v>29</v>
       </c>
-      <c r="C19" s="13" t="s">
+      <c r="C19" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="D19" s="13" t="s">
+      <c r="D19" s="35" t="s">
         <v>62</v>
       </c>
-      <c r="E19" s="13" t="s">
+      <c r="E19" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="F19" s="13" t="s">
+      <c r="F19" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="G19" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="H19" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="I19" s="24">
+      <c r="G19" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="H19" s="37" t="s">
+        <v>9</v>
+      </c>
+      <c r="I19" s="43">
         <v>5.79</v>
       </c>
-      <c r="J19" s="16"/>
+      <c r="J19" s="38" t="s">
+        <v>192</v>
+      </c>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="13"/>
@@ -1667,7 +1968,9 @@
       <c r="I20" s="24">
         <v>4.04</v>
       </c>
-      <c r="J20" s="16"/>
+      <c r="J20" s="16" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="13"/>
@@ -1695,7 +1998,9 @@
       <c r="I21" s="24">
         <v>3.53</v>
       </c>
-      <c r="J21" s="16"/>
+      <c r="J21" s="16" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="22" spans="1:10">
       <c r="A22" s="13"/>
@@ -1723,35 +2028,39 @@
       <c r="I22" s="24">
         <v>2.65</v>
       </c>
-      <c r="J22" s="16"/>
-    </row>
-    <row r="23" spans="1:10">
-      <c r="A23" s="13"/>
-      <c r="B23" s="13" t="s">
+      <c r="J22" s="16" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" s="41" customFormat="1" ht="48">
+      <c r="A23" s="35"/>
+      <c r="B23" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="C23" s="13" t="s">
+      <c r="C23" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="D23" s="13" t="s">
+      <c r="D23" s="35" t="s">
         <v>82</v>
       </c>
-      <c r="E23" s="13" t="s">
+      <c r="E23" s="35" t="s">
         <v>39</v>
       </c>
-      <c r="F23" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="G23" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="H23" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="I23" s="24">
+      <c r="F23" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="G23" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="H23" s="37" t="s">
+        <v>9</v>
+      </c>
+      <c r="I23" s="43">
         <v>2.14</v>
       </c>
-      <c r="J23" s="16"/>
+      <c r="J23" s="38" t="s">
+        <v>194</v>
+      </c>
     </row>
     <row r="24" spans="1:10">
       <c r="A24" s="13"/>
@@ -1779,7 +2088,9 @@
       <c r="I24" s="24">
         <v>2.02</v>
       </c>
-      <c r="J24" s="16"/>
+      <c r="J24" s="16" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="25" spans="1:10">
       <c r="A25" s="13"/>
@@ -1807,7 +2118,9 @@
       <c r="I25" s="24">
         <v>1.85</v>
       </c>
-      <c r="J25" s="16"/>
+      <c r="J25" s="16" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="26" spans="1:10">
       <c r="A26" s="14"/>
@@ -1835,7 +2148,9 @@
       <c r="I26" s="34">
         <v>1.68</v>
       </c>
-      <c r="J26" s="17"/>
+      <c r="J26" s="17" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="27" spans="1:10">
       <c r="A27" s="13" t="s">
@@ -1865,7 +2180,9 @@
       <c r="I27" s="24">
         <v>26.12</v>
       </c>
-      <c r="J27" s="16"/>
+      <c r="J27" s="16" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="28" spans="1:10">
       <c r="A28" s="13"/>
@@ -1893,7 +2210,9 @@
       <c r="I28" s="24">
         <v>16.75</v>
       </c>
-      <c r="J28" s="16"/>
+      <c r="J28" s="16" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="29" spans="1:10">
       <c r="A29" s="13"/>
@@ -1921,7 +2240,9 @@
       <c r="I29" s="24">
         <v>4.18</v>
       </c>
-      <c r="J29" s="16"/>
+      <c r="J29" s="16" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="30" spans="1:10">
       <c r="A30" s="13"/>
@@ -1949,7 +2270,9 @@
       <c r="I30" s="24">
         <v>3.25</v>
       </c>
-      <c r="J30" s="16"/>
+      <c r="J30" s="16" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="31" spans="1:10">
       <c r="A31" s="13"/>
@@ -1977,35 +2300,39 @@
       <c r="I31" s="24">
         <v>3.16</v>
       </c>
-      <c r="J31" s="16"/>
-    </row>
-    <row r="32" spans="1:10">
-      <c r="A32" s="13"/>
-      <c r="B32" s="13" t="s">
+      <c r="J31" s="16" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" s="41" customFormat="1" ht="32">
+      <c r="A32" s="35"/>
+      <c r="B32" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="C32" s="13" t="s">
+      <c r="C32" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="D32" s="13" t="s">
+      <c r="D32" s="35" t="s">
         <v>46</v>
       </c>
-      <c r="E32" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="F32" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="G32" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="H32" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="I32" s="24">
+      <c r="E32" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="F32" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="G32" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="H32" s="37" t="s">
+        <v>9</v>
+      </c>
+      <c r="I32" s="43">
         <v>3.01</v>
       </c>
-      <c r="J32" s="16"/>
+      <c r="J32" s="38" t="s">
+        <v>200</v>
+      </c>
     </row>
     <row r="33" spans="1:10">
       <c r="A33" s="13"/>
@@ -2033,7 +2360,9 @@
       <c r="I33" s="24">
         <v>2.69</v>
       </c>
-      <c r="J33" s="16"/>
+      <c r="J33" s="16" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="34" spans="1:10">
       <c r="A34" s="13"/>
@@ -2061,7 +2390,9 @@
       <c r="I34" s="24">
         <v>1.81</v>
       </c>
-      <c r="J34" s="16"/>
+      <c r="J34" s="16" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="35" spans="1:10">
       <c r="A35" s="13"/>
@@ -2089,7 +2420,9 @@
       <c r="I35" s="24">
         <v>1.51</v>
       </c>
-      <c r="J35" s="16"/>
+      <c r="J35" s="16" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="36" spans="1:10">
       <c r="A36" s="14"/>
@@ -2117,7 +2450,9 @@
       <c r="I36" s="34">
         <v>1.49</v>
       </c>
-      <c r="J36" s="16"/>
+      <c r="J36" s="14" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="37" spans="1:10">
       <c r="A37" s="13" t="s">
@@ -2147,7 +2482,9 @@
       <c r="I37" s="24">
         <v>17.760000000000002</v>
       </c>
-      <c r="J37" s="16"/>
+      <c r="J37" s="16" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="38" spans="1:10">
       <c r="A38" s="13"/>
@@ -2175,35 +2512,39 @@
       <c r="I38" s="24">
         <v>11.49</v>
       </c>
-      <c r="J38" s="16"/>
-    </row>
-    <row r="39" spans="1:10">
-      <c r="A39" s="13"/>
-      <c r="B39" s="13" t="s">
+      <c r="J38" s="16" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" s="48" customFormat="1" ht="32">
+      <c r="A39" s="45"/>
+      <c r="B39" s="45" t="s">
         <v>53</v>
       </c>
-      <c r="C39" s="13" t="s">
+      <c r="C39" s="45" t="s">
         <v>14</v>
       </c>
-      <c r="D39" s="13" t="s">
+      <c r="D39" s="45" t="s">
         <v>58</v>
       </c>
-      <c r="E39" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="F39" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="G39" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="H39" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="I39" s="24">
+      <c r="E39" s="45" t="s">
+        <v>9</v>
+      </c>
+      <c r="F39" s="45" t="s">
+        <v>9</v>
+      </c>
+      <c r="G39" s="45" t="s">
+        <v>9</v>
+      </c>
+      <c r="H39" s="46" t="s">
+        <v>9</v>
+      </c>
+      <c r="I39" s="50">
         <v>3.93</v>
       </c>
-      <c r="J39" s="16"/>
+      <c r="J39" s="47" t="s">
+        <v>199</v>
+      </c>
     </row>
     <row r="40" spans="1:10">
       <c r="A40" s="13"/>
@@ -2231,35 +2572,39 @@
       <c r="I40" s="24">
         <v>3.45</v>
       </c>
-      <c r="J40" s="16"/>
-    </row>
-    <row r="41" spans="1:10">
-      <c r="A41" s="13"/>
-      <c r="B41" s="13" t="s">
+      <c r="J40" s="16" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" s="41" customFormat="1" ht="48">
+      <c r="A41" s="35"/>
+      <c r="B41" s="35" t="s">
         <v>55</v>
       </c>
-      <c r="C41" s="13" t="s">
+      <c r="C41" s="35" t="s">
         <v>59</v>
       </c>
-      <c r="D41" s="13" t="s">
+      <c r="D41" s="35" t="s">
         <v>60</v>
       </c>
-      <c r="E41" s="13" t="s">
+      <c r="E41" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="F41" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="G41" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="H41" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="I41" s="24">
+      <c r="F41" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="G41" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="H41" s="37" t="s">
+        <v>9</v>
+      </c>
+      <c r="I41" s="43">
         <v>3.08</v>
       </c>
-      <c r="J41" s="16"/>
+      <c r="J41" s="38" t="s">
+        <v>198</v>
+      </c>
     </row>
     <row r="42" spans="1:10">
       <c r="A42" s="13"/>
@@ -2287,7 +2632,9 @@
       <c r="I42" s="24">
         <v>2.44</v>
       </c>
-      <c r="J42" s="16"/>
+      <c r="J42" s="16" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="43" spans="1:10">
       <c r="A43" s="13"/>
@@ -2315,7 +2662,9 @@
       <c r="I43" s="24">
         <v>2.33</v>
       </c>
-      <c r="J43" s="16"/>
+      <c r="J43" s="16" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="44" spans="1:10">
       <c r="A44" s="13"/>
@@ -2343,7 +2692,9 @@
       <c r="I44" s="24">
         <v>2.3199999999999998</v>
       </c>
-      <c r="J44" s="16"/>
+      <c r="J44" s="16" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="45" spans="1:10">
       <c r="A45" s="13"/>
@@ -2371,7 +2722,9 @@
       <c r="I45" s="24">
         <v>1.74</v>
       </c>
-      <c r="J45" s="16"/>
+      <c r="J45" s="16" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="14"/>
@@ -2399,7 +2752,9 @@
       <c r="I46" s="34">
         <v>1.69</v>
       </c>
-      <c r="J46" s="16"/>
+      <c r="J46" s="14" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="13" t="s">
@@ -2429,7 +2784,9 @@
       <c r="I47" s="24">
         <v>32.93</v>
       </c>
-      <c r="J47" s="16"/>
+      <c r="J47" s="16" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="48" spans="1:10">
       <c r="A48" s="13"/>
@@ -2457,7 +2814,9 @@
       <c r="I48" s="24">
         <v>14.64</v>
       </c>
-      <c r="J48" s="16"/>
+      <c r="J48" s="16" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="49" spans="1:10">
       <c r="A49" s="13"/>
@@ -2485,7 +2844,9 @@
       <c r="I49" s="24">
         <v>5</v>
       </c>
-      <c r="J49" s="16"/>
+      <c r="J49" s="16" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="50" spans="1:10">
       <c r="A50" s="13"/>
@@ -2513,7 +2874,9 @@
       <c r="I50" s="24">
         <v>3.19</v>
       </c>
-      <c r="J50" s="16"/>
+      <c r="J50" s="16" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="51" spans="1:10">
       <c r="A51" s="13"/>
@@ -2541,7 +2904,9 @@
       <c r="I51" s="24">
         <v>2.4500000000000002</v>
       </c>
-      <c r="J51" s="16"/>
+      <c r="J51" s="16" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="52" spans="1:10">
       <c r="A52" s="13"/>
@@ -2569,7 +2934,9 @@
       <c r="I52" s="24">
         <v>2.29</v>
       </c>
-      <c r="J52" s="16"/>
+      <c r="J52" s="16" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="53" spans="1:10">
       <c r="A53" s="13"/>
@@ -2597,7 +2964,9 @@
       <c r="I53" s="24">
         <v>2.0299999999999998</v>
       </c>
-      <c r="J53" s="16"/>
+      <c r="J53" s="16" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="54" spans="1:10">
       <c r="A54" s="13"/>
@@ -2625,7 +2994,9 @@
       <c r="I54" s="24">
         <v>1.76</v>
       </c>
-      <c r="J54" s="16"/>
+      <c r="J54" s="16" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="55" spans="1:10">
       <c r="A55" s="13"/>
@@ -2653,7 +3024,9 @@
       <c r="I55" s="24">
         <v>1.62</v>
       </c>
-      <c r="J55" s="16"/>
+      <c r="J55" s="16" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="56" spans="1:10">
       <c r="A56" s="14"/>
@@ -2681,7 +3054,9 @@
       <c r="I56" s="34">
         <v>1.58</v>
       </c>
-      <c r="J56" s="16"/>
+      <c r="J56" s="14" t="s">
+        <v>195</v>
+      </c>
     </row>
     <row r="57" spans="1:10">
       <c r="A57" s="13" t="s">
@@ -2711,7 +3086,9 @@
       <c r="I57" s="24">
         <v>17.260000000000002</v>
       </c>
-      <c r="J57" s="16"/>
+      <c r="J57" s="16" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="58" spans="1:10">
       <c r="A58" s="13"/>
@@ -2739,7 +3116,9 @@
       <c r="I58" s="24">
         <v>6.97</v>
       </c>
-      <c r="J58" s="16"/>
+      <c r="J58" s="16" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="59" spans="1:10">
       <c r="A59" s="13"/>
@@ -2767,7 +3146,9 @@
       <c r="I59" s="24">
         <v>6.53</v>
       </c>
-      <c r="J59" s="16"/>
+      <c r="J59" s="16" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="60" spans="1:10">
       <c r="A60" s="13"/>
@@ -2795,7 +3176,9 @@
       <c r="I60" s="24">
         <v>5.16</v>
       </c>
-      <c r="J60" s="16"/>
+      <c r="J60" s="16" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="61" spans="1:10">
       <c r="A61" s="13"/>
@@ -2823,7 +3206,9 @@
       <c r="I61" s="24">
         <v>5.14</v>
       </c>
-      <c r="J61" s="16"/>
+      <c r="J61" s="16" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="62" spans="1:10">
       <c r="A62" s="13"/>
@@ -2851,7 +3236,9 @@
       <c r="I62" s="24">
         <v>5.0199999999999996</v>
       </c>
-      <c r="J62" s="16"/>
+      <c r="J62" s="16" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="63" spans="1:10">
       <c r="A63" s="13"/>
@@ -2879,7 +3266,9 @@
       <c r="I63" s="24">
         <v>4.1500000000000004</v>
       </c>
-      <c r="J63" s="16"/>
+      <c r="J63" s="16" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="64" spans="1:10">
       <c r="A64" s="13"/>
@@ -2907,7 +3296,9 @@
       <c r="I64" s="24">
         <v>2.5099999999999998</v>
       </c>
-      <c r="J64" s="16"/>
+      <c r="J64" s="16" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="65" spans="1:10">
       <c r="A65" s="13"/>
@@ -2935,7 +3326,9 @@
       <c r="I65" s="24">
         <v>2.13</v>
       </c>
-      <c r="J65" s="16"/>
+      <c r="J65" s="16" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="66" spans="1:10">
       <c r="A66" s="14"/>
@@ -2963,7 +3356,9 @@
       <c r="I66" s="34">
         <v>2.09</v>
       </c>
-      <c r="J66" s="16"/>
+      <c r="J66" s="14" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="67" spans="1:10">
       <c r="A67" s="13" t="s">
@@ -2993,7 +3388,9 @@
       <c r="I67" s="24">
         <v>19.739999999999998</v>
       </c>
-      <c r="J67" s="16"/>
+      <c r="J67" s="16" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="68" spans="1:10">
       <c r="A68" s="13"/>
@@ -3021,7 +3418,9 @@
       <c r="I68" s="24">
         <v>17.91</v>
       </c>
-      <c r="J68" s="16"/>
+      <c r="J68" s="16" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="69" spans="1:10">
       <c r="A69" s="13"/>
@@ -3049,7 +3448,9 @@
       <c r="I69" s="24">
         <v>6.94</v>
       </c>
-      <c r="J69" s="16"/>
+      <c r="J69" s="16" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="70" spans="1:10">
       <c r="A70" s="13"/>
@@ -3077,7 +3478,9 @@
       <c r="I70" s="24">
         <v>4.42</v>
       </c>
-      <c r="J70" s="16"/>
+      <c r="J70" s="16" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="71" spans="1:10">
       <c r="A71" s="13"/>
@@ -3105,7 +3508,9 @@
       <c r="I71" s="24">
         <v>3.23</v>
       </c>
-      <c r="J71" s="16"/>
+      <c r="J71" s="16" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="72" spans="1:10">
       <c r="A72" s="13"/>
@@ -3133,7 +3538,9 @@
       <c r="I72" s="24">
         <v>2.89</v>
       </c>
-      <c r="J72" s="16"/>
+      <c r="J72" s="16" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="73" spans="1:10">
       <c r="A73" s="13"/>
@@ -3161,7 +3568,9 @@
       <c r="I73" s="24">
         <v>2.36</v>
       </c>
-      <c r="J73" s="16"/>
+      <c r="J73" s="16" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="74" spans="1:10">
       <c r="A74" s="13"/>
@@ -3189,7 +3598,9 @@
       <c r="I74" s="24">
         <v>2.19</v>
       </c>
-      <c r="J74" s="16"/>
+      <c r="J74" s="16" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="75" spans="1:10">
       <c r="A75" s="13"/>
@@ -3217,7 +3628,9 @@
       <c r="I75" s="24">
         <v>2.1800000000000002</v>
       </c>
-      <c r="J75" s="16"/>
+      <c r="J75" s="16" t="s">
+        <v>208</v>
+      </c>
     </row>
     <row r="76" spans="1:10">
       <c r="A76" s="14"/>
@@ -3245,7 +3658,9 @@
       <c r="I76" s="34">
         <v>1.69</v>
       </c>
-      <c r="J76" s="16"/>
+      <c r="J76" s="14" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="77" spans="1:10">
       <c r="A77" s="13" t="s">
@@ -3275,7 +3690,9 @@
       <c r="I77" s="24">
         <v>24.05</v>
       </c>
-      <c r="J77" s="16"/>
+      <c r="J77" s="16" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="78" spans="1:10">
       <c r="A78" s="13"/>
@@ -3303,7 +3720,9 @@
       <c r="I78" s="24">
         <v>9.4600000000000009</v>
       </c>
-      <c r="J78" s="16"/>
+      <c r="J78" s="16" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="79" spans="1:10">
       <c r="A79" s="13"/>
@@ -3331,7 +3750,9 @@
       <c r="I79" s="24">
         <v>5.05</v>
       </c>
-      <c r="J79" s="16"/>
+      <c r="J79" s="16" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="80" spans="1:10">
       <c r="A80" s="13"/>
@@ -3359,7 +3780,9 @@
       <c r="I80" s="24">
         <v>4.07</v>
       </c>
-      <c r="J80" s="16"/>
+      <c r="J80" s="16" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="81" spans="1:10">
       <c r="A81" s="13"/>
@@ -3387,7 +3810,9 @@
       <c r="I81" s="24">
         <v>3.35</v>
       </c>
-      <c r="J81" s="16"/>
+      <c r="J81" s="16" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="82" spans="1:10">
       <c r="A82" s="13"/>
@@ -3415,7 +3840,9 @@
       <c r="I82" s="24">
         <v>2.59</v>
       </c>
-      <c r="J82" s="16"/>
+      <c r="J82" s="16" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="83" spans="1:10">
       <c r="A83" s="13"/>
@@ -3443,7 +3870,9 @@
       <c r="I83" s="24">
         <v>2.0099999999999998</v>
       </c>
-      <c r="J83" s="16"/>
+      <c r="J83" s="16" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="84" spans="1:10">
       <c r="A84" s="13"/>
@@ -3471,7 +3900,9 @@
       <c r="I84" s="24">
         <v>1.83</v>
       </c>
-      <c r="J84" s="16"/>
+      <c r="J84" s="16" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="85" spans="1:10">
       <c r="A85" s="13"/>
@@ -3499,7 +3930,9 @@
       <c r="I85" s="24">
         <v>1.56</v>
       </c>
-      <c r="J85" s="16"/>
+      <c r="J85" s="16" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="86" spans="1:10">
       <c r="A86" s="14"/>
@@ -3527,7 +3960,9 @@
       <c r="I86" s="34">
         <v>1.54</v>
       </c>
-      <c r="J86" s="16"/>
+      <c r="J86" s="14" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="87" spans="1:10">
       <c r="A87" s="13" t="s">
@@ -3557,7 +3992,9 @@
       <c r="I87" s="24">
         <v>7.59</v>
       </c>
-      <c r="J87" s="16"/>
+      <c r="J87" s="16" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="88" spans="1:10">
       <c r="A88" s="13"/>
@@ -3585,7 +4022,9 @@
       <c r="I88" s="24">
         <v>6.09</v>
       </c>
-      <c r="J88" s="16"/>
+      <c r="J88" s="16" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="89" spans="1:10">
       <c r="A89" s="13"/>
@@ -3613,7 +4052,9 @@
       <c r="I89" s="24">
         <v>5.34</v>
       </c>
-      <c r="J89" s="16"/>
+      <c r="J89" s="16" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="90" spans="1:10">
       <c r="A90" s="13"/>
@@ -3641,7 +4082,9 @@
       <c r="I90" s="24">
         <v>4.0999999999999996</v>
       </c>
-      <c r="J90" s="16"/>
+      <c r="J90" s="16" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="91" spans="1:10">
       <c r="A91" s="13"/>
@@ -3669,7 +4112,9 @@
       <c r="I91" s="24">
         <v>3.82</v>
       </c>
-      <c r="J91" s="16"/>
+      <c r="J91" s="16" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="92" spans="1:10">
       <c r="A92" s="13"/>
@@ -3697,7 +4142,9 @@
       <c r="I92" s="24">
         <v>3.65</v>
       </c>
-      <c r="J92" s="16"/>
+      <c r="J92" s="16" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="93" spans="1:10">
       <c r="A93" s="13"/>
@@ -3725,7 +4172,9 @@
       <c r="I93" s="24">
         <v>3.64</v>
       </c>
-      <c r="J93" s="16"/>
+      <c r="J93" s="16" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="94" spans="1:10">
       <c r="A94" s="13"/>
@@ -3753,7 +4202,9 @@
       <c r="I94" s="24">
         <v>2.8</v>
       </c>
-      <c r="J94" s="16"/>
+      <c r="J94" s="16" t="s">
+        <v>196</v>
+      </c>
     </row>
     <row r="95" spans="1:10">
       <c r="A95" s="13"/>
@@ -3781,7 +4232,9 @@
       <c r="I95" s="24">
         <v>2.39</v>
       </c>
-      <c r="J95" s="16"/>
+      <c r="J95" s="16" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="96" spans="1:10">
       <c r="A96" s="14"/>
@@ -3809,7 +4262,9 @@
       <c r="I96" s="34">
         <v>1.91</v>
       </c>
-      <c r="J96" s="16"/>
+      <c r="J96" s="14" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="97" spans="1:10">
       <c r="A97" s="13" t="s">
@@ -3839,7 +4294,9 @@
       <c r="I97" s="24">
         <v>12.85</v>
       </c>
-      <c r="J97" s="16"/>
+      <c r="J97" s="16" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="98" spans="1:10">
       <c r="A98" s="13"/>
@@ -3867,7 +4324,9 @@
       <c r="I98" s="24">
         <v>11.61</v>
       </c>
-      <c r="J98" s="16"/>
+      <c r="J98" s="16" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="99" spans="1:10">
       <c r="A99" s="13"/>
@@ -3895,35 +4354,39 @@
       <c r="I99" s="24">
         <v>5.25</v>
       </c>
-      <c r="J99" s="16"/>
-    </row>
-    <row r="100" spans="1:10">
-      <c r="A100" s="13"/>
-      <c r="B100" s="13" t="s">
+      <c r="J99" s="16" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" s="41" customFormat="1" ht="64">
+      <c r="A100" s="35"/>
+      <c r="B100" s="35" t="s">
         <v>113</v>
       </c>
-      <c r="C100" s="13" t="s">
+      <c r="C100" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="D100" s="13" t="s">
+      <c r="D100" s="35" t="s">
         <v>82</v>
       </c>
-      <c r="E100" s="13" t="s">
+      <c r="E100" s="35" t="s">
         <v>114</v>
       </c>
-      <c r="F100" s="13" t="s">
+      <c r="F100" s="35" t="s">
         <v>115</v>
       </c>
-      <c r="G100" s="24" t="s">
-        <v>9</v>
-      </c>
-      <c r="H100" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="I100" s="24">
+      <c r="G100" s="43" t="s">
+        <v>9</v>
+      </c>
+      <c r="H100" s="37" t="s">
+        <v>9</v>
+      </c>
+      <c r="I100" s="43">
         <v>4.82</v>
       </c>
-      <c r="J100" s="16"/>
+      <c r="J100" s="38" t="s">
+        <v>197</v>
+      </c>
     </row>
     <row r="101" spans="1:10">
       <c r="A101" s="13"/>
@@ -3951,7 +4414,9 @@
       <c r="I101" s="24">
         <v>3</v>
       </c>
-      <c r="J101" s="16"/>
+      <c r="J101" s="16" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="102" spans="1:10">
       <c r="A102" s="13"/>
@@ -3979,7 +4444,9 @@
       <c r="I102" s="24">
         <v>2.46</v>
       </c>
-      <c r="J102" s="16"/>
+      <c r="J102" s="16" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="103" spans="1:10">
       <c r="A103" s="13"/>
@@ -4007,7 +4474,9 @@
       <c r="I103" s="24">
         <v>2.31</v>
       </c>
-      <c r="J103" s="16"/>
+      <c r="J103" s="16" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="104" spans="1:10">
       <c r="A104" s="13"/>
@@ -4035,7 +4504,9 @@
       <c r="I104" s="24">
         <v>2.29</v>
       </c>
-      <c r="J104" s="16"/>
+      <c r="J104" s="16" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="105" spans="1:10">
       <c r="A105" s="13"/>
@@ -4063,7 +4534,9 @@
       <c r="I105" s="24">
         <v>2.25</v>
       </c>
-      <c r="J105" s="16"/>
+      <c r="J105" s="16" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="106" spans="1:10">
       <c r="A106" s="14"/>
@@ -4091,7 +4564,9 @@
       <c r="I106" s="34">
         <v>1.76</v>
       </c>
-      <c r="J106" s="16"/>
+      <c r="J106" s="14" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="107" spans="1:10">
       <c r="A107" s="13" t="s">
@@ -4121,7 +4596,9 @@
       <c r="I107" s="24">
         <v>14.04</v>
       </c>
-      <c r="J107" s="16"/>
+      <c r="J107" s="16" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="108" spans="1:10">
       <c r="A108" s="13"/>
@@ -4149,7 +4626,9 @@
       <c r="I108" s="24">
         <v>8.8000000000000007</v>
       </c>
-      <c r="J108" s="16"/>
+      <c r="J108" s="16" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="109" spans="1:10">
       <c r="A109" s="13"/>
@@ -4177,7 +4656,9 @@
       <c r="I109" s="24">
         <v>8.01</v>
       </c>
-      <c r="J109" s="16"/>
+      <c r="J109" s="16" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="110" spans="1:10">
       <c r="A110" s="13"/>
@@ -4205,7 +4686,9 @@
       <c r="I110" s="24">
         <v>4.47</v>
       </c>
-      <c r="J110" s="16"/>
+      <c r="J110" s="16" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="111" spans="1:10">
       <c r="A111" s="13"/>
@@ -4233,7 +4716,9 @@
       <c r="I111" s="24">
         <v>3.52</v>
       </c>
-      <c r="J111" s="16"/>
+      <c r="J111" s="16" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="112" spans="1:10">
       <c r="A112" s="13"/>
@@ -4261,35 +4746,39 @@
       <c r="I112" s="24">
         <v>3.25</v>
       </c>
-      <c r="J112" s="16"/>
-    </row>
-    <row r="113" spans="1:10">
-      <c r="A113" s="13"/>
-      <c r="B113" s="13" t="s">
+      <c r="J112" s="16" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="113" spans="1:10" s="41" customFormat="1" ht="32">
+      <c r="A113" s="35"/>
+      <c r="B113" s="35" t="s">
         <v>120</v>
       </c>
-      <c r="C113" s="13" t="s">
+      <c r="C113" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="D113" s="13" t="s">
+      <c r="D113" s="35" t="s">
         <v>122</v>
       </c>
-      <c r="E113" s="13" t="s">
+      <c r="E113" s="35" t="s">
         <v>123</v>
       </c>
-      <c r="F113" s="13" t="s">
+      <c r="F113" s="35" t="s">
         <v>124</v>
       </c>
-      <c r="G113" s="31" t="s">
+      <c r="G113" s="52" t="s">
         <v>125</v>
       </c>
-      <c r="H113" s="28" t="s">
-        <v>9</v>
-      </c>
-      <c r="I113" s="24">
+      <c r="H113" s="51" t="s">
+        <v>9</v>
+      </c>
+      <c r="I113" s="43">
         <v>2.37</v>
       </c>
-      <c r="J113" s="16"/>
+      <c r="J113" s="38" t="s">
+        <v>202</v>
+      </c>
     </row>
     <row r="114" spans="1:10">
       <c r="A114" s="13"/>
@@ -4317,7 +4806,9 @@
       <c r="I114" s="24">
         <v>2.2999999999999998</v>
       </c>
-      <c r="J114" s="16"/>
+      <c r="J114" s="16" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="115" spans="1:10">
       <c r="A115" s="13"/>
@@ -4345,7 +4836,9 @@
       <c r="I115" s="24">
         <v>2.21</v>
       </c>
-      <c r="J115" s="16"/>
+      <c r="J115" s="16" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="116" spans="1:10">
       <c r="A116" s="14"/>
@@ -4373,7 +4866,9 @@
       <c r="I116" s="34">
         <v>2.14</v>
       </c>
-      <c r="J116" s="16"/>
+      <c r="J116" s="14" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="117" spans="1:10">
       <c r="A117" s="13" t="s">
@@ -4403,7 +4898,9 @@
       <c r="I117" s="24">
         <v>13.37</v>
       </c>
-      <c r="J117" s="16"/>
+      <c r="J117" s="16" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="118" spans="1:10">
       <c r="A118" s="13"/>
@@ -4431,7 +4928,9 @@
       <c r="I118" s="24">
         <v>12.76</v>
       </c>
-      <c r="J118" s="16"/>
+      <c r="J118" s="16" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="119" spans="1:10">
       <c r="A119" s="13"/>
@@ -4459,7 +4958,9 @@
       <c r="I119" s="24">
         <v>5.86</v>
       </c>
-      <c r="J119" s="16"/>
+      <c r="J119" s="16" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="120" spans="1:10">
       <c r="A120" s="13"/>
@@ -4487,7 +4988,9 @@
       <c r="I120" s="24">
         <v>5.56</v>
       </c>
-      <c r="J120" s="16"/>
+      <c r="J120" s="16" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="121" spans="1:10">
       <c r="A121" s="13"/>
@@ -4515,7 +5018,9 @@
       <c r="I121" s="24">
         <v>4.5199999999999996</v>
       </c>
-      <c r="J121" s="16"/>
+      <c r="J121" s="16" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="122" spans="1:10">
       <c r="A122" s="13"/>
@@ -4543,7 +5048,9 @@
       <c r="I122" s="24">
         <v>3.6</v>
       </c>
-      <c r="J122" s="16"/>
+      <c r="J122" s="16" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="123" spans="1:10">
       <c r="A123" s="13"/>
@@ -4571,7 +5078,9 @@
       <c r="I123" s="24">
         <v>3.54</v>
       </c>
-      <c r="J123" s="16"/>
+      <c r="J123" s="16" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="124" spans="1:10">
       <c r="A124" s="13"/>
@@ -4599,7 +5108,9 @@
       <c r="I124" s="24">
         <v>3.38</v>
       </c>
-      <c r="J124" s="16"/>
+      <c r="J124" s="16" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="125" spans="1:10">
       <c r="A125" s="13"/>
@@ -4627,7 +5138,9 @@
       <c r="I125" s="24">
         <v>3.35</v>
       </c>
-      <c r="J125" s="16"/>
+      <c r="J125" s="16" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="126" spans="1:10">
       <c r="A126" s="14"/>
@@ -4655,7 +5168,9 @@
       <c r="I126" s="34">
         <v>1.59</v>
       </c>
-      <c r="J126" s="16"/>
+      <c r="J126" s="14" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="127" spans="1:10">
       <c r="A127" s="13" t="s">
@@ -4685,7 +5200,9 @@
       <c r="I127" s="24">
         <v>24.85</v>
       </c>
-      <c r="J127" s="16"/>
+      <c r="J127" s="16" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="128" spans="1:10">
       <c r="A128" s="13"/>
@@ -4713,7 +5230,9 @@
       <c r="I128" s="24">
         <v>7.41</v>
       </c>
-      <c r="J128" s="16"/>
+      <c r="J128" s="16" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="129" spans="1:10">
       <c r="A129" s="13"/>
@@ -4741,7 +5260,9 @@
       <c r="I129" s="24">
         <v>6.04</v>
       </c>
-      <c r="J129" s="16"/>
+      <c r="J129" s="16" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="130" spans="1:10">
       <c r="A130" s="13"/>
@@ -4769,7 +5290,9 @@
       <c r="I130" s="24">
         <v>5.84</v>
       </c>
-      <c r="J130" s="16"/>
+      <c r="J130" s="16" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="131" spans="1:10">
       <c r="A131" s="13"/>
@@ -4797,7 +5320,9 @@
       <c r="I131" s="24">
         <v>2.82</v>
       </c>
-      <c r="J131" s="16"/>
+      <c r="J131" s="16" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="132" spans="1:10">
       <c r="A132" s="13"/>
@@ -4825,7 +5350,9 @@
       <c r="I132" s="24">
         <v>2.78</v>
       </c>
-      <c r="J132" s="16"/>
+      <c r="J132" s="16" t="s">
+        <v>203</v>
+      </c>
     </row>
     <row r="133" spans="1:10">
       <c r="A133" s="13"/>
@@ -4853,7 +5380,9 @@
       <c r="I133" s="24">
         <v>1.88</v>
       </c>
-      <c r="J133" s="16"/>
+      <c r="J133" s="16" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="134" spans="1:10">
       <c r="A134" s="13"/>
@@ -4881,7 +5410,9 @@
       <c r="I134" s="24">
         <v>1.8</v>
       </c>
-      <c r="J134" s="16"/>
+      <c r="J134" s="16" t="s">
+        <v>204</v>
+      </c>
     </row>
     <row r="135" spans="1:10">
       <c r="A135" s="13"/>
@@ -4909,7 +5440,9 @@
       <c r="I135" s="24">
         <v>1.77</v>
       </c>
-      <c r="J135" s="16"/>
+      <c r="J135" s="16" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="136" spans="1:10">
       <c r="A136" s="14"/>
@@ -4937,7 +5470,9 @@
       <c r="I136" s="34">
         <v>1.52</v>
       </c>
-      <c r="J136" s="16"/>
+      <c r="J136" s="14" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="137" spans="1:10">
       <c r="A137" s="13" t="s">
@@ -4967,7 +5502,9 @@
       <c r="I137" s="24">
         <v>16.809999999999999</v>
       </c>
-      <c r="J137" s="16"/>
+      <c r="J137" s="16" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="138" spans="1:10">
       <c r="A138" s="13"/>
@@ -4995,7 +5532,9 @@
       <c r="I138" s="24">
         <v>15.94</v>
       </c>
-      <c r="J138" s="16"/>
+      <c r="J138" s="16" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="139" spans="1:10">
       <c r="A139" s="13"/>
@@ -5023,7 +5562,9 @@
       <c r="I139" s="24">
         <v>7.16</v>
       </c>
-      <c r="J139" s="16"/>
+      <c r="J139" s="16" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="140" spans="1:10">
       <c r="A140" s="13"/>
@@ -5051,7 +5592,9 @@
       <c r="I140" s="24">
         <v>5.44</v>
       </c>
-      <c r="J140" s="16"/>
+      <c r="J140" s="16" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="141" spans="1:10">
       <c r="A141" s="13"/>
@@ -5079,7 +5622,9 @@
       <c r="I141" s="24">
         <v>3.84</v>
       </c>
-      <c r="J141" s="16"/>
+      <c r="J141" s="16" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="142" spans="1:10">
       <c r="A142" s="13"/>
@@ -5107,7 +5652,9 @@
       <c r="I142" s="24">
         <v>3.63</v>
       </c>
-      <c r="J142" s="16"/>
+      <c r="J142" s="16" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="143" spans="1:10">
       <c r="A143" s="13"/>
@@ -5135,7 +5682,9 @@
       <c r="I143" s="24">
         <v>3.15</v>
       </c>
-      <c r="J143" s="16"/>
+      <c r="J143" s="16" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="144" spans="1:10">
       <c r="A144" s="13"/>
@@ -5163,7 +5712,9 @@
       <c r="I144" s="24">
         <v>2.54</v>
       </c>
-      <c r="J144" s="16"/>
+      <c r="J144" s="16" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="145" spans="1:10">
       <c r="A145" s="13"/>
@@ -5191,7 +5742,9 @@
       <c r="I145" s="24">
         <v>2.17</v>
       </c>
-      <c r="J145" s="16"/>
+      <c r="J145" s="16" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="146" spans="1:10">
       <c r="A146" s="14"/>
@@ -5219,7 +5772,9 @@
       <c r="I146" s="34">
         <v>2.11</v>
       </c>
-      <c r="J146" s="16"/>
+      <c r="J146" s="14" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="147" spans="1:10">
       <c r="A147" s="13" t="s">
@@ -5249,7 +5804,9 @@
       <c r="I147" s="24">
         <v>21.56</v>
       </c>
-      <c r="J147" s="16"/>
+      <c r="J147" s="16" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="148" spans="1:10">
       <c r="A148" s="13"/>
@@ -5277,7 +5834,9 @@
       <c r="I148" s="24">
         <v>13.13</v>
       </c>
-      <c r="J148" s="16"/>
+      <c r="J148" s="16" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="149" spans="1:10">
       <c r="A149" s="13"/>
@@ -5305,35 +5864,39 @@
       <c r="I149" s="24">
         <v>5.9</v>
       </c>
-      <c r="J149" s="16"/>
-    </row>
-    <row r="150" spans="1:10">
-      <c r="A150" s="13"/>
-      <c r="B150" s="13" t="s">
+      <c r="J149" s="16" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="150" spans="1:10" s="41" customFormat="1" ht="32">
+      <c r="A150" s="35"/>
+      <c r="B150" s="35" t="s">
         <v>148</v>
       </c>
-      <c r="C150" s="13" t="s">
+      <c r="C150" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="D150" s="13" t="s">
+      <c r="D150" s="35" t="s">
         <v>46</v>
       </c>
-      <c r="E150" s="13" t="s">
+      <c r="E150" s="35" t="s">
         <v>151</v>
       </c>
-      <c r="F150" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="G150" s="24" t="s">
-        <v>9</v>
-      </c>
-      <c r="H150" s="28" t="s">
-        <v>9</v>
-      </c>
-      <c r="I150" s="24">
+      <c r="F150" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="G150" s="43" t="s">
+        <v>9</v>
+      </c>
+      <c r="H150" s="51" t="s">
+        <v>9</v>
+      </c>
+      <c r="I150" s="43">
         <v>4.67</v>
       </c>
-      <c r="J150" s="16"/>
+      <c r="J150" s="38" t="s">
+        <v>205</v>
+      </c>
     </row>
     <row r="151" spans="1:10">
       <c r="A151" s="13"/>
@@ -5361,7 +5924,9 @@
       <c r="I151" s="24">
         <v>3.68</v>
       </c>
-      <c r="J151" s="16"/>
+      <c r="J151" s="16" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="152" spans="1:10">
       <c r="A152" s="13"/>
@@ -5389,7 +5954,9 @@
       <c r="I152" s="24">
         <v>2.98</v>
       </c>
-      <c r="J152" s="16"/>
+      <c r="J152" s="16" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="153" spans="1:10">
       <c r="A153" s="13"/>
@@ -5417,7 +5984,9 @@
       <c r="I153" s="24">
         <v>2.34</v>
       </c>
-      <c r="J153" s="16"/>
+      <c r="J153" s="16" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="154" spans="1:10">
       <c r="A154" s="13"/>
@@ -5445,7 +6014,9 @@
       <c r="I154" s="24">
         <v>2.23</v>
       </c>
-      <c r="J154" s="16"/>
+      <c r="J154" s="16" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="155" spans="1:10">
       <c r="A155" s="13"/>
@@ -5473,7 +6044,9 @@
       <c r="I155" s="24">
         <v>2.23</v>
       </c>
-      <c r="J155" s="16"/>
+      <c r="J155" s="16" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="156" spans="1:10">
       <c r="A156" s="14"/>
@@ -5501,7 +6074,9 @@
       <c r="I156" s="34">
         <v>2.04</v>
       </c>
-      <c r="J156" s="16"/>
+      <c r="J156" s="14" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="157" spans="1:10">
       <c r="A157" s="13" t="s">
@@ -5531,7 +6106,9 @@
       <c r="I157" s="24">
         <v>16.71</v>
       </c>
-      <c r="J157" s="16"/>
+      <c r="J157" s="16" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="158" spans="1:10">
       <c r="A158" s="13"/>
@@ -5559,7 +6136,9 @@
       <c r="I158" s="24">
         <v>7.65</v>
       </c>
-      <c r="J158" s="16"/>
+      <c r="J158" s="16" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="159" spans="1:10">
       <c r="A159" s="13"/>
@@ -5587,7 +6166,9 @@
       <c r="I159" s="24">
         <v>5.07</v>
       </c>
-      <c r="J159" s="16"/>
+      <c r="J159" s="16" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="160" spans="1:10">
       <c r="A160" s="13"/>
@@ -5615,7 +6196,9 @@
       <c r="I160" s="24">
         <v>4.2699999999999996</v>
       </c>
-      <c r="J160" s="16"/>
+      <c r="J160" s="16" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="161" spans="1:10">
       <c r="A161" s="13"/>
@@ -5643,7 +6226,9 @@
       <c r="I161" s="24">
         <v>3.66</v>
       </c>
-      <c r="J161" s="16"/>
+      <c r="J161" s="16" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="162" spans="1:10">
       <c r="A162" s="13"/>
@@ -5671,7 +6256,9 @@
       <c r="I162" s="24">
         <v>2.83</v>
       </c>
-      <c r="J162" s="16"/>
+      <c r="J162" s="16" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="163" spans="1:10">
       <c r="A163" s="13"/>
@@ -5699,7 +6286,9 @@
       <c r="I163" s="24">
         <v>2.62</v>
       </c>
-      <c r="J163" s="16"/>
+      <c r="J163" s="16" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="164" spans="1:10">
       <c r="A164" s="13"/>
@@ -5727,7 +6316,9 @@
       <c r="I164" s="24">
         <v>2.25</v>
       </c>
-      <c r="J164" s="16"/>
+      <c r="J164" s="16" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="165" spans="1:10">
       <c r="A165" s="13"/>
@@ -5755,7 +6346,9 @@
       <c r="I165" s="24">
         <v>2.09</v>
       </c>
-      <c r="J165" s="16"/>
+      <c r="J165" s="16" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="166" spans="1:10">
       <c r="A166" s="14"/>
@@ -5783,7 +6376,9 @@
       <c r="I166" s="34">
         <v>1.64</v>
       </c>
-      <c r="J166" s="16"/>
+      <c r="J166" s="14" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="167" spans="1:10">
       <c r="A167" s="13" t="s">
@@ -5813,7 +6408,9 @@
       <c r="I167" s="24">
         <v>16.649999999999999</v>
       </c>
-      <c r="J167" s="16"/>
+      <c r="J167" s="16" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="168" spans="1:10">
       <c r="A168" s="13"/>
@@ -5841,7 +6438,9 @@
       <c r="I168" s="24">
         <v>11.58</v>
       </c>
-      <c r="J168" s="16"/>
+      <c r="J168" s="16" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="169" spans="1:10">
       <c r="A169" s="13"/>
@@ -5869,7 +6468,9 @@
       <c r="I169" s="24">
         <v>8.94</v>
       </c>
-      <c r="J169" s="16"/>
+      <c r="J169" s="16" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="170" spans="1:10">
       <c r="A170" s="13"/>
@@ -5897,7 +6498,9 @@
       <c r="I170" s="24">
         <v>5.31</v>
       </c>
-      <c r="J170" s="16"/>
+      <c r="J170" s="16" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="171" spans="1:10">
       <c r="A171" s="13"/>
@@ -5925,7 +6528,9 @@
       <c r="I171" s="24">
         <v>3.92</v>
       </c>
-      <c r="J171" s="16"/>
+      <c r="J171" s="16" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="172" spans="1:10">
       <c r="A172" s="13"/>
@@ -5953,7 +6558,9 @@
       <c r="I172" s="24">
         <v>3.77</v>
       </c>
-      <c r="J172" s="16"/>
+      <c r="J172" s="16" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="173" spans="1:10">
       <c r="A173" s="13"/>
@@ -5981,7 +6588,9 @@
       <c r="I173" s="24">
         <v>3.61</v>
       </c>
-      <c r="J173" s="16"/>
+      <c r="J173" s="16" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="174" spans="1:10">
       <c r="A174" s="13"/>
@@ -6009,7 +6618,9 @@
       <c r="I174" s="24">
         <v>3.12</v>
       </c>
-      <c r="J174" s="16"/>
+      <c r="J174" s="16" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="175" spans="1:10">
       <c r="A175" s="13"/>
@@ -6037,7 +6648,9 @@
       <c r="I175" s="24">
         <v>2.12</v>
       </c>
-      <c r="J175" s="16"/>
+      <c r="J175" s="16" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="176" spans="1:10">
       <c r="A176" s="14"/>
@@ -6065,7 +6678,9 @@
       <c r="I176" s="34">
         <v>1.64</v>
       </c>
-      <c r="J176" s="16"/>
+      <c r="J176" s="14" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="177" spans="1:10">
       <c r="A177" s="13" t="s">
@@ -6095,7 +6710,9 @@
       <c r="I177" s="24">
         <v>12.13</v>
       </c>
-      <c r="J177" s="16"/>
+      <c r="J177" s="16" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="178" spans="1:10">
       <c r="A178" s="13"/>
@@ -6123,7 +6740,9 @@
       <c r="I178" s="24">
         <v>11.69</v>
       </c>
-      <c r="J178" s="16"/>
+      <c r="J178" s="16" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="179" spans="1:10">
       <c r="A179" s="13"/>
@@ -6151,7 +6770,9 @@
       <c r="I179" s="24">
         <v>9.07</v>
       </c>
-      <c r="J179" s="16"/>
+      <c r="J179" s="16" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="180" spans="1:10">
       <c r="A180" s="13"/>
@@ -6179,7 +6800,9 @@
       <c r="I180" s="24">
         <v>5.79</v>
       </c>
-      <c r="J180" s="16"/>
+      <c r="J180" s="16" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="181" spans="1:10">
       <c r="A181" s="13"/>
@@ -6207,7 +6830,9 @@
       <c r="I181" s="24">
         <v>5.44</v>
       </c>
-      <c r="J181" s="16"/>
+      <c r="J181" s="16" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="182" spans="1:10">
       <c r="A182" s="13"/>
@@ -6235,7 +6860,9 @@
       <c r="I182" s="24">
         <v>4.3899999999999997</v>
       </c>
-      <c r="J182" s="16"/>
+      <c r="J182" s="16" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="183" spans="1:10">
       <c r="A183" s="13"/>
@@ -6263,7 +6890,9 @@
       <c r="I183" s="24">
         <v>3.79</v>
       </c>
-      <c r="J183" s="16"/>
+      <c r="J183" s="16" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="184" spans="1:10">
       <c r="A184" s="13"/>
@@ -6291,7 +6920,9 @@
       <c r="I184" s="24">
         <v>3.39</v>
       </c>
-      <c r="J184" s="16"/>
+      <c r="J184" s="16" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="185" spans="1:10">
       <c r="A185" s="13"/>
@@ -6319,7 +6950,9 @@
       <c r="I185" s="24">
         <v>2.96</v>
       </c>
-      <c r="J185" s="16"/>
+      <c r="J185" s="16" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="186" spans="1:10">
       <c r="A186" s="14"/>
@@ -6347,7 +6980,9 @@
       <c r="I186" s="34">
         <v>2.59</v>
       </c>
-      <c r="J186" s="16"/>
+      <c r="J186" s="14" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="187" spans="1:10">
       <c r="A187" s="13" t="s">
@@ -6377,7 +7012,9 @@
       <c r="I187" s="24">
         <v>18.96</v>
       </c>
-      <c r="J187" s="16"/>
+      <c r="J187" s="16" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="188" spans="1:10">
       <c r="A188" s="13"/>
@@ -6405,7 +7042,9 @@
       <c r="I188" s="24">
         <v>11.51</v>
       </c>
-      <c r="J188" s="16"/>
+      <c r="J188" s="16" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="189" spans="1:10">
       <c r="A189" s="13"/>
@@ -6433,7 +7072,9 @@
       <c r="I189" s="24">
         <v>3.99</v>
       </c>
-      <c r="J189" s="16"/>
+      <c r="J189" s="16" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="190" spans="1:10">
       <c r="A190" s="13"/>
@@ -6461,7 +7102,9 @@
       <c r="I190" s="24">
         <v>2.85</v>
       </c>
-      <c r="J190" s="16"/>
+      <c r="J190" s="16" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="191" spans="1:10">
       <c r="A191" s="13"/>
@@ -6489,7 +7132,9 @@
       <c r="I191" s="24">
         <v>2.73</v>
       </c>
-      <c r="J191" s="16"/>
+      <c r="J191" s="16" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="192" spans="1:10">
       <c r="A192" s="13"/>
@@ -6517,7 +7162,9 @@
       <c r="I192" s="24">
         <v>2.66</v>
       </c>
-      <c r="J192" s="16"/>
+      <c r="J192" s="16" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="193" spans="1:10">
       <c r="A193" s="13"/>
@@ -6545,7 +7192,9 @@
       <c r="I193" s="24">
         <v>2.65</v>
       </c>
-      <c r="J193" s="16"/>
+      <c r="J193" s="16" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="194" spans="1:10">
       <c r="A194" s="13"/>
@@ -6573,7 +7222,9 @@
       <c r="I194" s="24">
         <v>2.5299999999999998</v>
       </c>
-      <c r="J194" s="16"/>
+      <c r="J194" s="16" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="195" spans="1:10">
       <c r="A195" s="13"/>
@@ -6601,7 +7252,9 @@
       <c r="I195" s="24">
         <v>2.36</v>
       </c>
-      <c r="J195" s="16"/>
+      <c r="J195" s="16" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="196" spans="1:10">
       <c r="A196" s="14"/>
@@ -6629,7 +7282,9 @@
       <c r="I196" s="34">
         <v>2.3199999999999998</v>
       </c>
-      <c r="J196" s="16"/>
+      <c r="J196" s="14" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="197" spans="1:10">
       <c r="A197" s="13" t="s">
@@ -6659,7 +7314,9 @@
       <c r="I197" s="24">
         <v>14.57</v>
       </c>
-      <c r="J197" s="16"/>
+      <c r="J197" s="16" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="198" spans="1:10">
       <c r="A198" s="13"/>
@@ -6687,7 +7344,9 @@
       <c r="I198" s="24">
         <v>9.14</v>
       </c>
-      <c r="J198" s="16"/>
+      <c r="J198" s="16" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="199" spans="1:10">
       <c r="A199" s="13"/>
@@ -6715,7 +7374,9 @@
       <c r="I199" s="24">
         <v>5.07</v>
       </c>
-      <c r="J199" s="16"/>
+      <c r="J199" s="16" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="200" spans="1:10">
       <c r="A200" s="13"/>
@@ -6743,7 +7404,9 @@
       <c r="I200" s="24">
         <v>4.8499999999999996</v>
       </c>
-      <c r="J200" s="16"/>
+      <c r="J200" s="16" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="201" spans="1:10">
       <c r="A201" s="13"/>
@@ -6771,7 +7434,9 @@
       <c r="I201" s="24">
         <v>4.62</v>
       </c>
-      <c r="J201" s="16"/>
+      <c r="J201" s="16" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="202" spans="1:10">
       <c r="A202" s="13"/>
@@ -6799,7 +7464,9 @@
       <c r="I202" s="24">
         <v>4.17</v>
       </c>
-      <c r="J202" s="16"/>
+      <c r="J202" s="16" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="203" spans="1:10">
       <c r="A203" s="13"/>
@@ -6827,7 +7494,9 @@
       <c r="I203" s="24">
         <v>2.5099999999999998</v>
       </c>
-      <c r="J203" s="16"/>
+      <c r="J203" s="16" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="204" spans="1:10">
       <c r="A204" s="13"/>
@@ -6855,7 +7524,9 @@
       <c r="I204" s="24">
         <v>2.4300000000000002</v>
       </c>
-      <c r="J204" s="16"/>
+      <c r="J204" s="16" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="205" spans="1:10">
       <c r="A205" s="13"/>
@@ -6883,7 +7554,9 @@
       <c r="I205" s="24">
         <v>2.19</v>
       </c>
-      <c r="J205" s="16"/>
+      <c r="J205" s="16" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="206" spans="1:10">
       <c r="A206" s="14"/>
@@ -6911,7 +7584,9 @@
       <c r="I206" s="34">
         <v>2.1800000000000002</v>
       </c>
-      <c r="J206" s="16"/>
+      <c r="J206" s="14" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="207" spans="1:10">
       <c r="A207" s="13" t="s">
@@ -6941,7 +7616,9 @@
       <c r="I207" s="24">
         <v>21.99</v>
       </c>
-      <c r="J207" s="16"/>
+      <c r="J207" s="16" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="208" spans="1:10">
       <c r="A208" s="13"/>
@@ -6969,7 +7646,9 @@
       <c r="I208" s="24">
         <v>9.68</v>
       </c>
-      <c r="J208" s="16"/>
+      <c r="J208" s="16" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="209" spans="1:10">
       <c r="A209" s="13"/>
@@ -6997,7 +7676,9 @@
       <c r="I209" s="24">
         <v>4.53</v>
       </c>
-      <c r="J209" s="16"/>
+      <c r="J209" s="16" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="210" spans="1:10">
       <c r="A210" s="13"/>
@@ -7025,7 +7706,9 @@
       <c r="I210" s="24">
         <v>3.58</v>
       </c>
-      <c r="J210" s="16"/>
+      <c r="J210" s="16" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="211" spans="1:10">
       <c r="A211" s="13"/>
@@ -7053,7 +7736,9 @@
       <c r="I211" s="24">
         <v>3.02</v>
       </c>
-      <c r="J211" s="16"/>
+      <c r="J211" s="16" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="212" spans="1:10">
       <c r="A212" s="13"/>
@@ -7081,7 +7766,9 @@
       <c r="I212" s="24">
         <v>2.57</v>
       </c>
-      <c r="J212" s="16"/>
+      <c r="J212" s="16" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="213" spans="1:10">
       <c r="A213" s="13"/>
@@ -7109,7 +7796,9 @@
       <c r="I213" s="24">
         <v>2.42</v>
       </c>
-      <c r="J213" s="16"/>
+      <c r="J213" s="16" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="214" spans="1:10">
       <c r="A214" s="13"/>
@@ -7137,35 +7826,39 @@
       <c r="I214" s="24">
         <v>2.29</v>
       </c>
-      <c r="J214" s="16"/>
-    </row>
-    <row r="215" spans="1:10">
-      <c r="A215" s="13"/>
-      <c r="B215" s="13" t="s">
+      <c r="J214" s="16" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="215" spans="1:10" s="41" customFormat="1" ht="32">
+      <c r="A215" s="35"/>
+      <c r="B215" s="35" t="s">
         <v>182</v>
       </c>
-      <c r="C215" s="13" t="s">
+      <c r="C215" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="D215" s="13" t="s">
+      <c r="D215" s="35" t="s">
         <v>82</v>
       </c>
-      <c r="E215" s="13" t="s">
+      <c r="E215" s="35" t="s">
         <v>104</v>
       </c>
-      <c r="F215" s="13" t="s">
+      <c r="F215" s="35" t="s">
         <v>184</v>
       </c>
-      <c r="G215" s="31" t="s">
+      <c r="G215" s="52" t="s">
         <v>185</v>
       </c>
-      <c r="H215" s="19" t="s">
+      <c r="H215" s="42" t="s">
         <v>187</v>
       </c>
-      <c r="I215" s="24">
+      <c r="I215" s="43">
         <v>2.2799999999999998</v>
       </c>
-      <c r="J215" s="16"/>
+      <c r="J215" s="38" t="s">
+        <v>209</v>
+      </c>
     </row>
     <row r="216" spans="1:10">
       <c r="A216" s="14"/>
@@ -7193,7 +7886,9 @@
       <c r="I216" s="34">
         <v>2.25</v>
       </c>
-      <c r="J216" s="14"/>
+      <c r="J216" s="14" t="s">
+        <v>206</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="12">

</xml_diff>